<commit_message>
polish metadata, add protocol type
</commit_message>
<xml_diff>
--- a/templates/dataplant/next_generation_sequencing.xlsx
+++ b/templates/dataplant/next_generation_sequencing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26202"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/SWATE_templates/templates/dataplant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507F868-3D35-B842-A46A-AFF3AE3FD363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{D507F868-3D35-B842-A46A-AFF3AE3FD363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDAEB2C2-F22B-403C-B97E-82064D92F826}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1320" windowWidth="26600" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="1320" windowWidth="26600" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="next_generation_sequencing" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,157 +49,76 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{43048E28-13C8-4707-A267-458F0BB83DD3}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The unique identifier of this template. It will be auto generated.
 Reply:
     id=145a3170-58e0-4b1c-b790-b71e5d0084cc</t>
-        </r>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{3AD04854-3877-45BC-A82A-51D936F9F82B}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The name of the Swate template.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{61AD5462-E737-4882-9EB1-AFBF8E46E93D}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The current version of this template in SemVer notation.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{5BCC1A13-8A08-46F4-99F8-CEBB11FC7321}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The description of this template. Use few sentences for succinctness.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{38CCB781-FD67-405F-BAD3-3127F335DB6E}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{AEAB3864-E499-4A40-9029-1C723FC9C719}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{82E8C057-6792-41FB-B6E8-3DD65DA28864}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{08881E4A-A459-45A6-8C3D-9927A9BF8294}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     A list of all tags associated with this template. Tags are realized as Terms.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{AE6443B4-1634-4B60-B96F-79D530853534}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The author(s) of this template.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -204,11 +126,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>Source Name</t>
   </si>
   <si>
+    <t>Protocol Type</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000161)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000161)</t>
+  </si>
+  <si>
     <t>Parameter [library layout]</t>
   </si>
   <si>
@@ -248,6 +179,15 @@
     <t>Raw Data File</t>
   </si>
   <si>
+    <t>assay protocol</t>
+  </si>
+  <si>
+    <t>DPBO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000177</t>
+  </si>
+  <si>
     <t>Id</t>
   </si>
   <si>
@@ -257,7 +197,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>next generation sequencing</t>
+    <t>Next Generation Sequencing</t>
   </si>
   <si>
     <t>Version</t>
@@ -269,6 +209,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Minimal template for next generation sequencing</t>
+  </si>
+  <si>
     <t>Organisation</t>
   </si>
   <si>
@@ -299,6 +242,12 @@
     <t>Tags</t>
   </si>
   <si>
+    <t>RNASeq</t>
+  </si>
+  <si>
+    <t>NGS</t>
+  </si>
+  <si>
     <t>Tags Term Accession Number</t>
   </si>
   <si>
@@ -338,7 +287,13 @@
     <t>Authors Affiliation</t>
   </si>
   <si>
+    <t>CEPLAS (https://ror.org/034waa237)</t>
+  </si>
+  <si>
     <t>Authors ORCID</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-9021-3197</t>
   </si>
   <si>
     <t>Authors Role</t>
@@ -354,7 +309,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,8 +325,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,6 +363,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FCDB3"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -485,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -514,11 +481,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -554,6 +525,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -575,10 +555,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EBBC1B10-A713-48E0-A6B6-D4CBE9288AD1}" name="annotationTableBlackImpala62" displayName="annotationTableBlackImpala62" ref="A1:N2" totalsRowShown="0">
-  <autoFilter ref="A1:N2" xr:uid="{EBBC1B10-A713-48E0-A6B6-D4CBE9288AD1}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EBBC1B10-A713-48E0-A6B6-D4CBE9288AD1}" name="annotationTableBlackImpala62" displayName="annotationTableBlackImpala62" ref="A1:Q2" totalsRowShown="0">
+  <autoFilter ref="A1:Q2" xr:uid="{EBBC1B10-A713-48E0-A6B6-D4CBE9288AD1}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{27DFE68E-DA51-4833-B237-D242408BF4D1}" name="Source Name"/>
+    <tableColumn id="15" xr3:uid="{9E6FA45B-688D-4B02-AC87-8D302AA4FF2E}" name="Protocol Type" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{1805CEE2-BDE4-48F5-89D9-EBC651463B24}" name="Term Source REF (DPBO:1000161)" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{F8FB80A1-0398-44FF-B240-938A8BF5DF14}" name="Term Accession Number (DPBO:1000161)" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{AFD7872E-0791-4598-8054-B7CF12529D82}" name="Parameter [library layout]" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{02E58DFF-1743-4EBD-958D-8D2BC98F25D2}" name="Term Source REF (DPBO:0000015)" dataDxfId="10"/>
     <tableColumn id="5" xr3:uid="{2B61A330-118A-426C-B9D6-15417FBEFADB}" name="Term Accession Number (DPBO:0000015)" dataDxfId="9"/>
@@ -929,50 +912,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="41.1640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="45.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="45.1640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="57.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="57.6640625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.5" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.1640625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="45.6640625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.5" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="45.1640625" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="57.7109375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.42578125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="42.140625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="45.7109375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.42578125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="38.140625" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="45.140625" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1014,6 +997,26 @@
       </c>
       <c r="N1" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="B2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1026,191 +1029,212 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6B2A7A-A06E-432C-91AE-70B45AC16592}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.1640625" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.95">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.95">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="50.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.95">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.95">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B27" s="9"/>
     </row>

</xml_diff>

<commit_message>
replaced nfdi4pso terms in next generation sequencing template
</commit_message>
<xml_diff>
--- a/templates/dataplant/next_generation_sequencing.xlsx
+++ b/templates/dataplant/next_generation_sequencing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nfdi4plant-my.sharepoint.com/personal/brilhaus_nfdi4plants_org/Documents/Swate-templates_git/templates/dataplant/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\ARCs und SWATE\ersatz von nfdi4pso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{D507F868-3D35-B842-A46A-AFF3AE3FD363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3B23AFF-95ED-EA42-9364-E4280956AECE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D104E19-F617-4B86-8A26-EC03081F8759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="1000" windowWidth="26600" windowHeight="14020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="next_generation_sequencing" sheetId="1" r:id="rId1"/>
@@ -46,157 +46,76 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{43048E28-13C8-4707-A267-458F0BB83DD3}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The unique identifier of this template. It will be auto generated.
-Reply:
+Antwort:
     id=145a3170-58e0-4b1c-b790-b71e5d0084cc</t>
-        </r>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{3AD04854-3877-45BC-A82A-51D936F9F82B}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate template.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{61AD5462-E737-4882-9EB1-AFBF8E46E93D}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The current version of this template in SemVer notation.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{5BCC1A13-8A08-46F4-99F8-CEBB11FC7321}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The description of this template. Use few sentences for succinctness.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{38CCB781-FD67-405F-BAD3-3127F335DB6E}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{AEAB3864-E499-4A40-9029-1C723FC9C719}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{82E8C057-6792-41FB-B6E8-3DD65DA28864}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{08881E4A-A459-45A6-8C3D-9927A9BF8294}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all tags associated with this template. Tags are realized as Terms.</t>
-        </r>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{AE6443B4-1634-4B60-B96F-79D530853534}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The author(s) of this template.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -204,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>Source Name</t>
   </si>
@@ -227,33 +146,6 @@
     <t>Term Accession Number (DPBO:0000015)</t>
   </si>
   <si>
-    <t>Parameter [Library strategy]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000035)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000035)</t>
-  </si>
-  <si>
-    <t>Parameter [Library preparation kit]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000037)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000037)</t>
-  </si>
-  <si>
-    <t>Parameter [Next generation sequencing instrument model]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:0000040)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000040)</t>
-  </si>
-  <si>
     <t>Raw Data File</t>
   </si>
   <si>
@@ -380,7 +272,37 @@
     <t>NCIT</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>Parameter [library strategy]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000035)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000035)</t>
+  </si>
+  <si>
+    <t>Parameter [library preparation kit]</t>
+  </si>
+  <si>
+    <t>Term Source REF (GENEPIO:0000085)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (GENEPIO:0000085)</t>
+  </si>
+  <si>
+    <t>Parameter [next generation sequencing instrument model]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000040)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000040)</t>
   </si>
 </sst>
 </file>
@@ -565,35 +487,35 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -643,15 +565,15 @@
     <tableColumn id="3" xr3:uid="{AFD7872E-0791-4598-8054-B7CF12529D82}" name="Parameter [library layout]" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{02E58DFF-1743-4EBD-958D-8D2BC98F25D2}" name="Term Source REF (DPBO:0000015)" dataDxfId="10"/>
     <tableColumn id="5" xr3:uid="{2B61A330-118A-426C-B9D6-15417FBEFADB}" name="Term Accession Number (DPBO:0000015)" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{31494651-A1ED-42BF-90C4-24AEEE9887DC}" name="Parameter [Library strategy]" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{D35BD4FB-835D-48DD-93C6-80AC65B37846}" name="Term Source REF (NFDI4PSO:0000035)" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{54639D5C-B4BF-43AA-BFA0-5F0BFA0ACC16}" name="Term Accession Number (NFDI4PSO:0000035)" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{AE80912D-9B14-43E6-99FE-B2BF18ECD252}" name="Parameter [Library preparation kit]" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{25B6C26C-09BB-4A0D-8AEF-EBFD3EE29540}" name="Term Source REF (NFDI4PSO:0000037)" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{A042CD48-9063-49A6-A046-7D8F5C4DC24B}" name="Term Accession Number (NFDI4PSO:0000037)" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{6E423EDB-D912-4F8E-9E4B-BAC9D0A43953}" name="Parameter [Next generation sequencing instrument model]" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{702B5B29-45CA-4911-9C56-F7BD6D4FCD8F}" name="Term Source REF (NFDI4PSO:0000040)" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{777C5356-00A6-44E4-8C66-F4B049875CF2}" name="Term Accession Number (NFDI4PSO:0000040)" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{C55D949E-169D-4ADA-9B2D-C2E0BFD132C2}" name="Parameter [library strategy]" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{4739FC42-0BEE-486E-8054-D54EE29DCC51}" name="Term Source REF (DPBO:0000035)" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{88C23753-1DD0-48F9-8CCE-000BA3256133}" name="Term Accession Number (DPBO:0000035)" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{AC76D1C3-DB9C-44D0-B92F-8C7771920C5B}" name="Parameter [library preparation kit]" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{F3C9B6A6-F7CE-4256-8418-DF683842F77D}" name="Term Source REF (GENEPIO:0000085)" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{C4000BAB-7926-472D-BC86-1EAD582E0693}" name="Term Accession Number (GENEPIO:0000085)" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{F216D752-E949-4615-8E33-724C44D9F5AD}" name="Parameter [next generation sequencing instrument model]" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{DE232661-D1C8-4EA9-B71C-881E86501E1B}" name="Term Source REF (DPBO:0000040)" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{96B2830E-7E6D-47A6-BB01-DC39EAD1989E}" name="Term Accession Number (DPBO:0000040)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A1C32613-CD5E-4162-8042-94756F5A21F6}" name="Raw Data File"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -659,7 +581,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -988,52 +910,70 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="651" row="2">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{421CEE82-072C-418C-B77D-80C886FEC50D}">
+  <we:reference id="5d6f5462-3401-48ec-9406-d12882e9ad83" version="0.6.2.0" store="\\DESKTOP-99AC8GC\Users\Stella Eggels\Downloads\swate-win" storeType="Filesystem"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="41.1640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="41.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="45.1640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="57.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="57.6640625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.5" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.1640625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5546875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="41" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="53.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.44140625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="42.109375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="45.6640625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.5" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.44140625" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="38.1640625" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="45.1640625" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="45.109375" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1056,45 +996,70 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="D2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>19</v>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1110,210 +1075,210 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.1640625" customWidth="1"/>
-    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B23" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="B27" s="9"/>
     </row>

</xml_diff>

<commit_message>
harmonize curated template names and match file names
</commit_message>
<xml_diff>
--- a/templates/dataplant/next_generation_sequencing.xlsx
+++ b/templates/dataplant/next_generation_sequencing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A174032-5CCD-4ACF-9630-BFF80741A85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73109157-06D6-4F1E-A355-2776A4960F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Source Name</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>OBI:0000070</t>
+  </si>
+  <si>
+    <t>Next generation sequencing</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1084,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,7 +1107,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>